<commit_message>
make changes to supplementary files
</commit_message>
<xml_diff>
--- a/supplement/Table_S3_Core_GO_Enrichment.xlsx
+++ b/supplement/Table_S3_Core_GO_Enrichment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psaroudakis/tomato-rna-meta/supplement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8734E7F4-F95B-3141-BF5A-0B689162944C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6FF994-C929-C148-9A5D-113DA6021B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" activeTab="5"/>
+    <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="15940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="heat_upregulated" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,9 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="1.4_core_response_drought_downregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_drought_downregulated_GOs.csv" comma="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="1.4_core_response_drought_downregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_drought_downregulated_GOs.csv" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -46,8 +46,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="1.4_core_response_drought_upregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_drought_upregulated_GOs.csv" comma="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="1.4_core_response_drought_upregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_drought_upregulated_GOs.csv" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -59,8 +59,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="1.4_core_response_heat_downregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_heat_downregulated_GOs.csv" comma="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="1.4_core_response_heat_downregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_heat_downregulated_GOs.csv" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -72,8 +72,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="1.4_core_response_salt_downregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_salt_downregulated_GOs.csv" comma="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="1.4_core_response_salt_downregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_salt_downregulated_GOs.csv" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -85,8 +85,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="1.4_core_response_salt_upregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_salt_upregulated_GOs.csv" comma="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="1.4_core_response_salt_upregulated_GOs" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/psaroudakis/tomato-rna-meta/1_core_response/output/1.4_core_response_salt_upregulated_GOs.csv" comma="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="290">
   <si>
     <t>GO.ID</t>
   </si>
@@ -969,12 +969,15 @@
   </si>
   <si>
     <t>carbohydrate biosynthetic process</t>
+  </si>
+  <si>
+    <t>(No significantly enriched terms were found for this gene set)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1452,9 +1455,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1514,29 +1518,29 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1.4_core_response_heat_downregulated_GOs" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="1.4_core_response_heat_downregulated_GOs" connectionId="3" xr16:uid="{00000000-0016-0000-0100-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1.4_core_response_drought_upregulated_GOs" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="1.4_core_response_drought_upregulated_GOs" connectionId="2" xr16:uid="{00000000-0016-0000-0200-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1.4_core_response_drought_downregulated_GOs" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="1.4_core_response_drought_downregulated_GOs" connectionId="1" xr16:uid="{00000000-0016-0000-0300-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1.4_core_response_salt_upregulated_GOs" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="1.4_core_response_salt_upregulated_GOs" connectionId="5" xr16:uid="{00000000-0016-0000-0400-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="1.4_core_response_salt_downregulated_GOs" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="1.4_core_response_salt_downregulated_GOs" connectionId="4" xr16:uid="{00000000-0016-0000-0500-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1574,7 +1578,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1680,7 +1684,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1822,14 +1826,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2624,10 +2628,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2640,7 +2646,7 @@
     <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2661,6 +2667,11 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -2669,7 +2680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3588,10 +3599,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3604,7 +3617,7 @@
     <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3625,6 +3638,11 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="2" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3633,7 +3651,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5518,10 +5536,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>